<commit_message>
modificando plantilla y agregando bcrypt
</commit_message>
<xml_diff>
--- a/src/main/resources/plantilla_carga_masiva.xlsx
+++ b/src/main/resources/plantilla_carga_masiva.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto\MachMillenium\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5121A40-80CC-4A5C-A027-31E48F86695D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E8B621-DE5E-455E-9A9E-884350336F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{C41CCF0B-61AF-43A0-88E7-CE1C140B00CA}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C41CCF0B-61AF-43A0-88E7-CE1C140B00CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Personal" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
   <si>
     <t>Nombre</t>
   </si>
@@ -67,16 +67,33 @@
   </si>
   <si>
     <t>Administrador</t>
+  </si>
+  <si>
+    <t>Correo</t>
+  </si>
+  <si>
+    <t>admin@mach.com</t>
+  </si>
+  <si>
+    <t>ingeniero@mach.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -99,13 +116,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -438,10 +458,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F42165BF-21DC-4F2D-9D39-01CFE143CBDE}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -449,9 +469,10 @@
     <col min="1" max="1" width="14" customWidth="1"/>
     <col min="2" max="2" width="14.77734375" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" customWidth="1"/>
+    <col min="5" max="5" width="30.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -464,8 +485,11 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
+      <c r="E1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -478,8 +502,11 @@
       <c r="D2" t="b">
         <v>1</v>
       </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -492,8 +519,15 @@
       <c r="D3" t="b">
         <v>0</v>
       </c>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{A17BDE33-0969-47E4-A872-7DE87EC6DC05}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{65D3BD46-748E-4375-8F57-098E4509B684}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
agregando rol y defaults
</commit_message>
<xml_diff>
--- a/src/main/resources/plantilla_carga_masiva.xlsx
+++ b/src/main/resources/plantilla_carga_masiva.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto\MachMillenium\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57E8B621-DE5E-455E-9A9E-884350336F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47A03766-5C70-47D0-9A9D-00C14D241833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{C41CCF0B-61AF-43A0-88E7-CE1C140B00CA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="16440" windowHeight="28320" xr2:uid="{C41CCF0B-61AF-43A0-88E7-CE1C140B00CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Personal" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
   <si>
     <t>Nombre</t>
   </si>
@@ -76,6 +76,24 @@
   </si>
   <si>
     <t>ingeniero@mach.com</t>
+  </si>
+  <si>
+    <t>Rol</t>
+  </si>
+  <si>
+    <t>Usuario Operativo</t>
+  </si>
+  <si>
+    <t>Mario Jimenez</t>
+  </si>
+  <si>
+    <t>V-4958314</t>
+  </si>
+  <si>
+    <t>gerente@mach.com</t>
+  </si>
+  <si>
+    <t>Gerente de Proyecto</t>
   </si>
 </sst>
 </file>
@@ -458,10 +476,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F42165BF-21DC-4F2D-9D39-01CFE143CBDE}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -470,9 +488,10 @@
     <col min="2" max="2" width="14.77734375" customWidth="1"/>
     <col min="3" max="3" width="15.88671875" customWidth="1"/>
     <col min="5" max="5" width="30.5546875" customWidth="1"/>
+    <col min="6" max="6" width="23.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,8 +507,11 @@
       <c r="E1" t="s">
         <v>10</v>
       </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -505,8 +527,11 @@
       <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
+      <c r="F2" t="s">
+        <v>9</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -522,11 +547,40 @@
       <c r="E3" s="1" t="s">
         <v>12</v>
       </c>
+      <c r="F3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" t="s">
+        <v>18</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No aceptado" error="Elija uno de los valores pre-establecidos" sqref="F2:F12518" xr:uid="{F2B36EF2-C789-4E38-94F3-F959D0A6DBE9}">
+      <formula1>"Administrador,Gerente de Proyecto,Usuario Operativo"</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{A17BDE33-0969-47E4-A872-7DE87EC6DC05}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{65D3BD46-748E-4375-8F57-098E4509B684}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{FD561AB3-2DCB-4537-9967-5A85BED9684A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
mejorando preguntas de seguridad
</commit_message>
<xml_diff>
--- a/src/main/resources/plantilla_carga_masiva.xlsx
+++ b/src/main/resources/plantilla_carga_masiva.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proyecto\MachMillenium\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10F9D919-C784-4B34-B51F-021D17FDE9F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77684A7-F667-4E56-AC4B-E128E4B32C2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{C41CCF0B-61AF-43A0-88E7-CE1C140B00CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{C41CCF0B-61AF-43A0-88E7-CE1C140B00CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Personal" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
   <si>
     <t>Nombre</t>
   </si>
@@ -96,15 +96,6 @@
     <t>Gerente de Proyecto</t>
   </si>
   <si>
-    <t>Pregunta seguridad 1: ¿En qué ciudad naciste?</t>
-  </si>
-  <si>
-    <t>Pregunta seguridad 2: ¿Cuál es tu color favorito?</t>
-  </si>
-  <si>
-    <t>Pregunta seguridad 3: ¿Cuál es tu comida favorita?</t>
-  </si>
-  <si>
     <t>Fecha de Fin de contrato (DD/MM/AAAA)</t>
   </si>
   <si>
@@ -135,17 +126,38 @@
     <t>PASTA</t>
   </si>
   <si>
-    <t>ARROZ</t>
-  </si>
-  <si>
-    <t>HUEVO</t>
+    <t>Pregunta seguridad 1</t>
+  </si>
+  <si>
+    <t>Respuesta de la pregunta 1</t>
+  </si>
+  <si>
+    <t>Pregunta seguridad 2</t>
+  </si>
+  <si>
+    <t>Respuesta de la pregunta 2</t>
+  </si>
+  <si>
+    <t>Pregunta seguridad 3</t>
+  </si>
+  <si>
+    <t>Respuesta de la pregunta 3</t>
+  </si>
+  <si>
+    <t>¿En que ciudad naciste?</t>
+  </si>
+  <si>
+    <t>¿Color favorito?</t>
+  </si>
+  <si>
+    <t>¿Comida favorita?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -157,6 +169,12 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -527,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F42165BF-21DC-4F2D-9D39-01CFE143CBDE}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,9 +563,12 @@
     <col min="8" max="8" width="45.28515625" customWidth="1"/>
     <col min="9" max="9" width="45.85546875" customWidth="1"/>
     <col min="10" max="10" width="47.5703125" customWidth="1"/>
+    <col min="11" max="11" width="30.5703125" customWidth="1"/>
+    <col min="12" max="12" width="30.140625" customWidth="1"/>
+    <col min="13" max="13" width="35.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -567,19 +588,28 @@
         <v>13</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="H1" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
-        <v>21</v>
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M1" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -599,19 +629,28 @@
         <v>9</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="H2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
         <v>25</v>
       </c>
-      <c r="I2" t="s">
+      <c r="L2" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" t="s">
         <v>28</v>
       </c>
-      <c r="J2" t="s">
-        <v>31</v>
-      </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -631,19 +670,28 @@
         <v>14</v>
       </c>
       <c r="G3" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="H3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
       <c r="J3" t="s">
-        <v>32</v>
+        <v>36</v>
+      </c>
+      <c r="K3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" t="s">
+        <v>37</v>
+      </c>
+      <c r="M3" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>15</v>
       </c>
@@ -666,16 +714,26 @@
         <v>45637</v>
       </c>
       <c r="H4" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="I4" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="J4" t="s">
-        <v>33</v>
+        <v>36</v>
+      </c>
+      <c r="K4" t="s">
+        <v>26</v>
+      </c>
+      <c r="L4" t="s">
+        <v>37</v>
+      </c>
+      <c r="M4" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="No aceptado" error="Elija uno de los valores pre-establecidos" sqref="F2:F12518" xr:uid="{F2B36EF2-C789-4E38-94F3-F959D0A6DBE9}">
       <formula1>"Administrador,Gerente de Proyecto,Usuario Operativo"</formula1>

</xml_diff>